<commit_message>
Commit required changes for tool functionality
</commit_message>
<xml_diff>
--- a/tests/analysis/analysis.xlsx
+++ b/tests/analysis/analysis.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,7 +492,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>setAspect, init, evaluate, nowMs</t>
+          <t>init, evaluate, nowMs, setAspect</t>
         </is>
       </c>
       <c r="E2" t="b">
@@ -520,14 +520,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>setAspect, evaluate, update, isHealthy, isOccupied, nowMs</t>
+          <t>setAspect, nowMs, isOccupied, update, evaluateControllerLogic, isHealthy</t>
         </is>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -604,7 +604,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>simultaneously, writeLamp</t>
+          <t>writeLamp, simultaneously</t>
         </is>
       </c>
       <c r="E6" t="b">
@@ -632,7 +632,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>readRawClear, configure</t>
+          <t>configure, readRawClear</t>
         </is>
       </c>
       <c r="E7" t="b">
@@ -716,7 +716,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>else, digitalWrite</t>
+          <t>digitalWrite, else</t>
         </is>
       </c>
       <c r="E10" t="b">
@@ -801,12 +801,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>evaluate</t>
+          <t>computeControllerFresh</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>src\logic\Interlocking.cpp</t>
+          <t>src\logic\ControllerHelpers.cpp</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -819,6 +819,58 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>evaluateControllerLogic</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>src\logic\ControllerLogic.cpp</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>cpp</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>evaluate, computeControllerFresh</t>
+        </is>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>evaluate</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>src\logic\Interlocking.cpp</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>cpp</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -833,7 +885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -865,7 +917,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>setAspect, init, evaluate, nowMs</t>
+          <t>init, evaluate, nowMs, setAspect</t>
         </is>
       </c>
     </row>
@@ -877,7 +929,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>setAspect, evaluate, update, isHealthy, isOccupied, nowMs</t>
+          <t>setAspect, nowMs, isOccupied, update, evaluateControllerLogic, isHealthy</t>
         </is>
       </c>
     </row>
@@ -913,7 +965,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>simultaneously, writeLamp</t>
+          <t>writeLamp, simultaneously</t>
         </is>
       </c>
     </row>
@@ -925,7 +977,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>readRawClear, configure</t>
+          <t>configure, readRawClear</t>
         </is>
       </c>
     </row>
@@ -961,7 +1013,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>else, digitalWrite</t>
+          <t>digitalWrite, else</t>
         </is>
       </c>
     </row>
@@ -992,10 +1044,30 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>computeControllerFresh</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>evaluateControllerLogic</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>evaluate, computeControllerFresh</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>evaluate</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1008,7 +1080,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1072,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1203,22 +1275,66 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>src\logic\ControllerHelpers.cpp</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>src\logic\ControllerLogic.cpp</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>src\logic\Interlocking.cpp, src\logic\ControllerHelpers.cpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>src\logic\Interlocking.cpp</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1258,55 +1374,55 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ArduinoGpio</t>
+          <t>TrackCircuitInput</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HARDWARE</t>
+          <t>MIXED</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MockGpio</t>
+          <t>BlockController</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HARDWARE</t>
+          <t>MIXED</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BlockController</t>
+          <t>ArduinoGpio</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MIXED</t>
+          <t>HARDWARE</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SignalHead</t>
+          <t>MockGpio</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MIXED</t>
+          <t>HARDWARE</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TrackCircuitInput</t>
+          <t>SignalHead</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">

</xml_diff>

<commit_message>
Update project files with latest changes
</commit_message>
<xml_diff>
--- a/tests/analysis/analysis.xlsx
+++ b/tests/analysis/analysis.xlsx
@@ -492,7 +492,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>init, evaluate, nowMs, setAspect</t>
+          <t>setAspect, nowMs, init, evaluate</t>
         </is>
       </c>
       <c r="E2" t="b">
@@ -520,7 +520,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>setAspect, nowMs, isOccupied, update, evaluateControllerLogic, isHealthy</t>
+          <t>nowMs, isOccupied, evaluateControllerLogic, update, setAspect, isHealthy</t>
         </is>
       </c>
       <c r="E3" t="b">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -632,11 +632,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>configure, readRawClear</t>
+          <t>readRawClear, configure</t>
         </is>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -688,7 +688,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>pinMode, else</t>
+          <t>else, pinMode</t>
         </is>
       </c>
       <c r="E9" t="b">
@@ -716,7 +716,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>digitalWrite, else</t>
+          <t>else, digitalWrite</t>
         </is>
       </c>
       <c r="E10" t="b">
@@ -917,7 +917,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>init, evaluate, nowMs, setAspect</t>
+          <t>setAspect, nowMs, init, evaluate</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>setAspect, nowMs, isOccupied, update, evaluateControllerLogic, isHealthy</t>
+          <t>nowMs, isOccupied, evaluateControllerLogic, update, setAspect, isHealthy</t>
         </is>
       </c>
     </row>
@@ -977,7 +977,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>configure, readRawClear</t>
+          <t>readRawClear, configure</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>pinMode, else</t>
+          <t>else, pinMode</t>
         </is>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>digitalWrite, else</t>
+          <t>else, digitalWrite</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -1185,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>src\logic\Interlocking.cpp, src\logic\ControllerHelpers.cpp</t>
+          <t>src\logic\ControllerHelpers.cpp, src\logic\Interlocking.cpp</t>
         </is>
       </c>
     </row>
@@ -1386,48 +1386,48 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BlockController</t>
+          <t>MockGpio</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MIXED</t>
+          <t>HARDWARE</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ArduinoGpio</t>
+          <t>SignalHead</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HARDWARE</t>
+          <t>MIXED</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MockGpio</t>
+          <t>BlockController</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>HARDWARE</t>
+          <t>MIXED</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SignalHead</t>
+          <t>ArduinoGpio</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MIXED</t>
+          <t>HARDWARE</t>
         </is>
       </c>
     </row>

</xml_diff>